<commit_message>
add number of invalid dashed lines
</commit_message>
<xml_diff>
--- a/data/study2canada_indicatorsCAMs_long.xlsx
+++ b/data/study2canada_indicatorsCAMs_long.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>CAM_ID</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>num_edges_dashed</t>
+  </si>
+  <si>
+    <t>num_edges_invaliddashed</t>
   </si>
   <si>
     <t>reciprocity</t>
@@ -207,6 +210,9 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -252,33 +258,36 @@
         <v>0.0</v>
       </c>
       <c r="O2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P2" t="n">
         <v>0.636363636363636</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>0.274239991433064</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>-0.285903789141444</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>10.0</v>
       </c>
-      <c r="S2" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U2" t="n">
         <v>2.27272727272727</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>0.628515495302329</v>
       </c>
-      <c r="V2" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X2" t="n">
         <v>-0.153846153846154</v>
       </c>
-      <c r="X2" t="n">
+      <c r="Y2" t="n">
         <v>-0.615384615384615</v>
       </c>
     </row>
@@ -326,33 +335,36 @@
         <v>2.0</v>
       </c>
       <c r="O3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P3" t="n">
         <v>0.588235294117647</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>-0.241456069693291</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>-0.52550294607051</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>9.0</v>
       </c>
-      <c r="S3" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T3" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="U3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V3" t="n">
         <v>0.391755537032627</v>
       </c>
-      <c r="V3" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X3" t="n">
         <v>-0.5</v>
       </c>
-      <c r="X3" t="n">
+      <c r="Y3" t="n">
         <v>-0.916666666666667</v>
       </c>
     </row>
@@ -400,33 +412,36 @@
         <v>11.0</v>
       </c>
       <c r="O4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="P4" t="n">
         <v>0.545454545454545</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>-0.183154007382219</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>-0.261676811621462</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>13.0</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>5.0</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>2.3030303030303</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>0.528938384926935</v>
       </c>
-      <c r="V4" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X4" t="n">
         <v>0.294117647058824</v>
       </c>
-      <c r="X4" t="n">
+      <c r="Y4" t="n">
         <v>0.941176470588235</v>
       </c>
     </row>
@@ -474,33 +489,36 @@
         <v>6.0</v>
       </c>
       <c r="O5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="P5" t="n">
         <v>0.842105263157895</v>
       </c>
-      <c r="P5" t="n">
-        <v>0.0</v>
-      </c>
       <c r="Q5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R5" t="n">
         <v>0.343303281162798</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>11.0</v>
       </c>
-      <c r="S5" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U5" t="n">
         <v>2.89473684210526</v>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
         <v>0.050418724139669</v>
       </c>
-      <c r="V5" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X5" t="n">
         <v>-0.75</v>
       </c>
-      <c r="X5" t="n">
+      <c r="Y5" t="n">
         <v>-2.25</v>
       </c>
     </row>
@@ -548,33 +566,36 @@
         <v>8.0</v>
       </c>
       <c r="O6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P6" t="n">
         <v>0.5</v>
       </c>
-      <c r="P6" t="n">
+      <c r="Q6" t="n">
         <v>-0.181568259800641</v>
       </c>
-      <c r="Q6" t="n">
-        <v>0.0</v>
-      </c>
       <c r="R6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S6" t="n">
         <v>8.0</v>
       </c>
-      <c r="S6" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U6" t="n">
         <v>2.125</v>
       </c>
-      <c r="U6" t="n">
+      <c r="V6" t="n">
         <v>0.342284451659452</v>
       </c>
-      <c r="V6" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X6" t="n">
         <v>0.4</v>
       </c>
-      <c r="X6" t="n">
+      <c r="Y6" t="n">
         <v>0.9</v>
       </c>
     </row>
@@ -622,33 +643,36 @@
         <v>0.0</v>
       </c>
       <c r="O7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q7" t="n">
         <v>-0.0158172231985941</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="R7" t="n">
         <v>-0.521306818181818</v>
       </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
         <v>7.0</v>
       </c>
-      <c r="S7" t="n">
-        <v>3.0</v>
-      </c>
       <c r="T7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U7" t="n">
         <v>2.29411764705882</v>
       </c>
-      <c r="U7" t="n">
+      <c r="V7" t="n">
         <v>0.817352472089314</v>
       </c>
-      <c r="V7" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X7" t="n">
         <v>-0.416666666666667</v>
       </c>
-      <c r="X7" t="n">
+      <c r="Y7" t="n">
         <v>-1.33333333333333</v>
       </c>
     </row>
@@ -696,33 +720,36 @@
         <v>0.0</v>
       </c>
       <c r="O8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P8" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>-0.758721223333605</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
         <v>-0.286609097982238</v>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>6.0</v>
       </c>
-      <c r="S8" t="n">
-        <v>3.0</v>
-      </c>
       <c r="T8" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="U8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V8" t="n">
         <v>0.52113695128401</v>
       </c>
-      <c r="V8" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X8" t="n">
         <v>-0.222222222222222</v>
       </c>
-      <c r="X8" t="n">
+      <c r="Y8" t="n">
         <v>-0.666666666666667</v>
       </c>
     </row>
@@ -770,33 +797,36 @@
         <v>4.0</v>
       </c>
       <c r="O9" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="P9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q9" t="n">
         <v>-0.5625</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="R9" t="n">
         <v>-0.739130434782609</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>5.0</v>
       </c>
-      <c r="S9" t="n">
-        <v>3.0</v>
-      </c>
       <c r="T9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U9" t="n">
         <v>1.4</v>
       </c>
-      <c r="U9" t="n">
+      <c r="V9" t="n">
         <v>0.73125</v>
       </c>
-      <c r="V9" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W9" t="n">
         <v>0.0</v>
       </c>
       <c r="X9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y9" t="n">
         <v>-0.333333333333333</v>
       </c>
     </row>
@@ -844,33 +874,36 @@
         <v>0.0</v>
       </c>
       <c r="O10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q10" t="n">
         <v>-0.285714285714285</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="R10" t="n">
         <v>-0.445026178010471</v>
       </c>
-      <c r="R10" t="n">
+      <c r="S10" t="n">
         <v>6.0</v>
       </c>
-      <c r="S10" t="n">
-        <v>3.0</v>
-      </c>
       <c r="T10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U10" t="n">
         <v>2.25</v>
       </c>
-      <c r="U10" t="n">
+      <c r="V10" t="n">
         <v>0.446151996151996</v>
       </c>
-      <c r="V10" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X10" t="n">
         <v>-0.125</v>
       </c>
-      <c r="X10" t="n">
+      <c r="Y10" t="n">
         <v>-0.375</v>
       </c>
     </row>
@@ -918,33 +951,36 @@
         <v>5.0</v>
       </c>
       <c r="O11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="P11" t="n">
         <v>0.857142857142857</v>
       </c>
-      <c r="P11" t="n">
+      <c r="Q11" t="n">
         <v>-0.0242893083778635</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="R11" t="n">
         <v>-0.407778228948779</v>
       </c>
-      <c r="R11" t="n">
+      <c r="S11" t="n">
         <v>8.0</v>
       </c>
-      <c r="S11" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U11" t="n">
         <v>1.89285714285714</v>
       </c>
-      <c r="U11" t="n">
+      <c r="V11" t="n">
         <v>0.39874826059456</v>
       </c>
-      <c r="V11" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X11" t="n">
         <v>-0.25</v>
       </c>
-      <c r="X11" t="n">
+      <c r="Y11" t="n">
         <v>-0.5</v>
       </c>
     </row>
@@ -992,33 +1028,36 @@
         <v>0.0</v>
       </c>
       <c r="O12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q12" t="n">
         <v>0.298245614035088</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="R12" t="n">
         <v>-0.079646017699115</v>
       </c>
-      <c r="R12" t="n">
+      <c r="S12" t="n">
         <v>16.0</v>
       </c>
-      <c r="S12" t="n">
+      <c r="T12" t="n">
         <v>8.0</v>
       </c>
-      <c r="T12" t="n">
-        <v>2.0</v>
-      </c>
       <c r="U12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V12" t="n">
         <v>0.22507348353418</v>
       </c>
-      <c r="V12" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X12" t="n">
         <v>-0.208333333333333</v>
       </c>
-      <c r="X12" t="n">
+      <c r="Y12" t="n">
         <v>-0.75</v>
       </c>
     </row>
@@ -1066,33 +1105,36 @@
         <v>0.0</v>
       </c>
       <c r="O13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P13" t="n">
         <v>0.973684210526316</v>
       </c>
-      <c r="P13" t="n">
+      <c r="Q13" t="n">
         <v>-0.0252507782774128</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="R13" t="n">
         <v>0.0352713296168676</v>
       </c>
-      <c r="R13" t="n">
+      <c r="S13" t="n">
         <v>9.0</v>
       </c>
-      <c r="S13" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T13" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U13" t="n">
         <v>2.05263157894737</v>
       </c>
-      <c r="U13" t="n">
+      <c r="V13" t="n">
         <v>0.299714943422809</v>
       </c>
-      <c r="V13" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X13" t="n">
         <v>-0.142857142857143</v>
       </c>
-      <c r="X13" t="n">
+      <c r="Y13" t="n">
         <v>-0.380952380952381</v>
       </c>
     </row>
@@ -1140,33 +1182,36 @@
         <v>3.0</v>
       </c>
       <c r="O14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P14" t="n">
         <v>0.315789473684211</v>
       </c>
-      <c r="P14" t="n">
+      <c r="Q14" t="n">
         <v>0.259778102573499</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="R14" t="n">
         <v>-0.423793568418581</v>
       </c>
-      <c r="R14" t="n">
+      <c r="S14" t="n">
         <v>8.0</v>
       </c>
-      <c r="S14" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T14" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U14" t="n">
         <v>1.94736842105263</v>
       </c>
-      <c r="U14" t="n">
+      <c r="V14" t="n">
         <v>0.662100981283072</v>
       </c>
-      <c r="V14" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W14" t="n">
         <v>0.0</v>
       </c>
       <c r="X14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y14" t="n">
         <v>0.142857142857143</v>
       </c>
     </row>
@@ -1214,33 +1259,36 @@
         <v>2.0</v>
       </c>
       <c r="O15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P15" t="n">
         <v>0.75</v>
       </c>
-      <c r="P15" t="n">
+      <c r="Q15" t="n">
         <v>-0.590075770593729</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="R15" t="n">
         <v>-0.692240552994768</v>
       </c>
-      <c r="R15" t="n">
+      <c r="S15" t="n">
         <v>10.0</v>
       </c>
-      <c r="S15" t="n">
+      <c r="T15" t="n">
         <v>5.0</v>
       </c>
-      <c r="T15" t="n">
-        <v>2.0</v>
-      </c>
       <c r="U15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V15" t="n">
         <v>0.34565114639043</v>
       </c>
-      <c r="V15" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X15" t="n">
         <v>-0.173913043478261</v>
       </c>
-      <c r="X15" t="n">
+      <c r="Y15" t="n">
         <v>-0.565217391304348</v>
       </c>
     </row>
@@ -1291,30 +1339,33 @@
         <v>0.0</v>
       </c>
       <c r="P16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q16" t="n">
         <v>-0.263523138347365</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="R16" t="n">
         <v>-0.458831467741123</v>
       </c>
-      <c r="R16" t="n">
+      <c r="S16" t="n">
         <v>9.0</v>
       </c>
-      <c r="S16" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U16" t="n">
         <v>2.3</v>
       </c>
-      <c r="U16" t="n">
+      <c r="V16" t="n">
         <v>0.640451388888889</v>
       </c>
-      <c r="V16" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W16" t="n">
         <v>0.0</v>
       </c>
       <c r="X16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y16" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -1362,33 +1413,36 @@
         <v>2.0</v>
       </c>
       <c r="O17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P17" t="n">
         <v>0.6</v>
       </c>
-      <c r="P17" t="n">
+      <c r="Q17" t="n">
         <v>0.763762615825972</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="R17" t="n">
         <v>-0.210675242900096</v>
       </c>
-      <c r="R17" t="n">
+      <c r="S17" t="n">
         <v>10.0</v>
       </c>
-      <c r="S17" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T17" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U17" t="n">
         <v>2.3</v>
       </c>
-      <c r="U17" t="n">
+      <c r="V17" t="n">
         <v>0.576602564102564</v>
       </c>
-      <c r="V17" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X17" t="n">
         <v>-0.428571428571429</v>
       </c>
-      <c r="X17" t="n">
+      <c r="Y17" t="n">
         <v>-0.714285714285714</v>
       </c>
     </row>
@@ -1436,33 +1490,36 @@
         <v>5.0</v>
       </c>
       <c r="O18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P18" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="P18" t="n">
+      <c r="Q18" t="n">
         <v>0.516397779494323</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="R18" t="n">
         <v>-0.421520915881641</v>
       </c>
-      <c r="R18" t="n">
+      <c r="S18" t="n">
         <v>12.0</v>
       </c>
-      <c r="S18" t="n">
+      <c r="T18" t="n">
         <v>6.0</v>
       </c>
-      <c r="T18" t="n">
-        <v>2.0</v>
-      </c>
       <c r="U18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V18" t="n">
         <v>0.434700387194293</v>
       </c>
-      <c r="V18" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X18" t="n">
         <v>-0.454545454545455</v>
       </c>
-      <c r="X18" t="n">
+      <c r="Y18" t="n">
         <v>-1.04545454545455</v>
       </c>
     </row>
@@ -1510,33 +1567,36 @@
         <v>6.0</v>
       </c>
       <c r="O19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="P19" t="n">
         <v>0.6875</v>
       </c>
-      <c r="P19" t="n">
+      <c r="Q19" t="n">
         <v>0.0482000706339824</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="R19" t="n">
         <v>-0.00998254580392466</v>
       </c>
-      <c r="R19" t="n">
+      <c r="S19" t="n">
         <v>12.0</v>
       </c>
-      <c r="S19" t="n">
+      <c r="T19" t="n">
         <v>6.0</v>
       </c>
-      <c r="T19" t="n">
-        <v>2.0</v>
-      </c>
       <c r="U19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V19" t="n">
         <v>0.379341380593057</v>
       </c>
-      <c r="V19" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X19" t="n">
         <v>-0.157894736842105</v>
       </c>
-      <c r="X19" t="n">
+      <c r="Y19" t="n">
         <v>-0.894736842105263</v>
       </c>
     </row>
@@ -1584,33 +1644,36 @@
         <v>1.0</v>
       </c>
       <c r="O20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P20" t="n">
         <v>0.307692307692308</v>
       </c>
-      <c r="P20" t="n">
+      <c r="Q20" t="n">
         <v>0.200308404192444</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="R20" t="n">
         <v>-0.570087712549569</v>
       </c>
-      <c r="R20" t="n">
+      <c r="S20" t="n">
         <v>12.0</v>
       </c>
-      <c r="S20" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T20" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U20" t="n">
         <v>2.92307692307692</v>
       </c>
-      <c r="U20" t="n">
+      <c r="V20" t="n">
         <v>0.40547970391951</v>
       </c>
-      <c r="V20" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X20" t="n">
         <v>0.0909090909090909</v>
       </c>
-      <c r="X20" t="n">
+      <c r="Y20" t="n">
         <v>0.0909090909090909</v>
       </c>
     </row>
@@ -1658,33 +1721,36 @@
         <v>0.0</v>
       </c>
       <c r="O21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q21" t="n">
         <v>-0.718213058419244</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="R21" t="n">
         <v>-0.375</v>
       </c>
-      <c r="R21" t="n">
+      <c r="S21" t="n">
         <v>8.0</v>
       </c>
-      <c r="S21" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T21" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="U21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V21" t="n">
         <v>0.591394335511982</v>
       </c>
-      <c r="V21" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X21" t="n">
         <v>0.125</v>
       </c>
-      <c r="X21" t="n">
+      <c r="Y21" t="n">
         <v>0.625</v>
       </c>
     </row>
@@ -1732,33 +1798,36 @@
         <v>2.0</v>
       </c>
       <c r="O22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P22" t="n">
         <v>0.869565217391304</v>
       </c>
-      <c r="P22" t="n">
+      <c r="Q22" t="n">
         <v>-0.490475318171924</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="R22" t="n">
         <v>0.0534215967583193</v>
       </c>
-      <c r="R22" t="n">
+      <c r="S22" t="n">
         <v>8.0</v>
       </c>
-      <c r="S22" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T22" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U22" t="n">
         <v>1.95652173913043</v>
       </c>
-      <c r="U22" t="n">
+      <c r="V22" t="n">
         <v>0.537979422566003</v>
       </c>
-      <c r="V22" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X22" t="n">
         <v>-0.571428571428571</v>
       </c>
-      <c r="X22" t="n">
+      <c r="Y22" t="n">
         <v>-0.928571428571429</v>
       </c>
     </row>
@@ -1806,33 +1875,36 @@
         <v>6.0</v>
       </c>
       <c r="O23" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="P23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q23" t="n">
         <v>-0.220338983050847</v>
       </c>
-      <c r="Q23" t="n">
+      <c r="R23" t="n">
         <v>-0.362162162162162</v>
       </c>
-      <c r="R23" t="n">
+      <c r="S23" t="n">
         <v>10.0</v>
       </c>
-      <c r="S23" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T23" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U23" t="n">
         <v>2.44444444444444</v>
       </c>
-      <c r="U23" t="n">
+      <c r="V23" t="n">
         <v>0.603053968623022</v>
       </c>
-      <c r="V23" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X23" t="n">
         <v>0.444444444444444</v>
       </c>
-      <c r="X23" t="n">
+      <c r="Y23" t="n">
         <v>1.11111111111111</v>
       </c>
     </row>
@@ -1880,33 +1952,36 @@
         <v>3.0</v>
       </c>
       <c r="O24" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="P24" t="n">
         <v>0.4</v>
       </c>
-      <c r="P24" t="n">
+      <c r="Q24" t="n">
         <v>-0.0297350516725031</v>
       </c>
-      <c r="Q24" t="n">
+      <c r="R24" t="n">
         <v>-0.349689303090118</v>
       </c>
-      <c r="R24" t="n">
+      <c r="S24" t="n">
         <v>10.0</v>
       </c>
-      <c r="S24" t="n">
+      <c r="T24" t="n">
         <v>5.0</v>
       </c>
-      <c r="T24" t="n">
+      <c r="U24" t="n">
         <v>2.05</v>
       </c>
-      <c r="U24" t="n">
+      <c r="V24" t="n">
         <v>0.295764499851474</v>
       </c>
-      <c r="V24" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X24" t="n">
         <v>-0.307692307692308</v>
       </c>
-      <c r="X24" t="n">
+      <c r="Y24" t="n">
         <v>-0.692307692307692</v>
       </c>
     </row>
@@ -1954,33 +2029,36 @@
         <v>2.0</v>
       </c>
       <c r="O25" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P25" t="n">
         <v>0.428571428571429</v>
       </c>
-      <c r="P25" t="n">
-        <v>0.0</v>
-      </c>
       <c r="Q25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R25" t="n">
         <v>-0.188342700875221</v>
       </c>
-      <c r="R25" t="n">
-        <v>4.0</v>
-      </c>
       <c r="S25" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="T25" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="U25" t="n">
         <v>2.14285714285714</v>
       </c>
-      <c r="U25" t="n">
+      <c r="V25" t="n">
         <v>0.522321428571428</v>
       </c>
-      <c r="V25" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X25" t="n">
         <v>-0.333333333333333</v>
       </c>
-      <c r="X25" t="n">
+      <c r="Y25" t="n">
         <v>-0.666666666666667</v>
       </c>
     </row>
@@ -2031,30 +2109,33 @@
         <v>0.0</v>
       </c>
       <c r="P26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q26" t="n">
         <v>0.585366132238558</v>
       </c>
-      <c r="Q26" t="n">
+      <c r="R26" t="n">
         <v>-0.540738070435875</v>
       </c>
-      <c r="R26" t="n">
+      <c r="S26" t="n">
         <v>10.0</v>
       </c>
-      <c r="S26" t="n">
+      <c r="T26" t="n">
         <v>5.0</v>
       </c>
-      <c r="T26" t="n">
-        <v>2.0</v>
-      </c>
       <c r="U26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V26" t="n">
         <v>0.326528838637392</v>
       </c>
-      <c r="V26" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X26" t="n">
         <v>0.363636363636364</v>
       </c>
-      <c r="X26" t="n">
+      <c r="Y26" t="n">
         <v>0.636363636363636</v>
       </c>
     </row>
@@ -2102,33 +2183,36 @@
         <v>4.0</v>
       </c>
       <c r="O27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P27" t="n">
         <v>0.222222222222222</v>
       </c>
-      <c r="P27" t="n">
+      <c r="Q27" t="n">
         <v>0.104742905504447</v>
       </c>
-      <c r="Q27" t="n">
+      <c r="R27" t="n">
         <v>-0.15095978794505</v>
       </c>
-      <c r="R27" t="n">
+      <c r="S27" t="n">
         <v>12.0</v>
       </c>
-      <c r="S27" t="n">
+      <c r="T27" t="n">
         <v>6.0</v>
       </c>
-      <c r="T27" t="n">
-        <v>2.0</v>
-      </c>
       <c r="U27" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V27" t="n">
         <v>0.52294040571033</v>
       </c>
-      <c r="V27" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W27" t="n">
         <v>0.0</v>
       </c>
       <c r="X27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y27" t="n">
         <v>0.411764705882353</v>
       </c>
     </row>
@@ -2176,33 +2260,36 @@
         <v>2.0</v>
       </c>
       <c r="O28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P28" t="n">
         <v>0.4</v>
       </c>
-      <c r="P28" t="n">
+      <c r="Q28" t="n">
         <v>-0.563173311782862</v>
       </c>
-      <c r="Q28" t="n">
+      <c r="R28" t="n">
         <v>-0.527010142562539</v>
       </c>
-      <c r="R28" t="n">
+      <c r="S28" t="n">
         <v>6.0</v>
       </c>
-      <c r="S28" t="n">
-        <v>2.0</v>
-      </c>
       <c r="T28" t="n">
         <v>2.0</v>
       </c>
       <c r="U28" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V28" t="n">
         <v>0.952083333333334</v>
       </c>
-      <c r="V28" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W28" t="n">
         <v>0.0</v>
       </c>
       <c r="X28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y28" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2250,33 +2337,36 @@
         <v>11.0</v>
       </c>
       <c r="O29" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="P29" t="n">
         <v>0.628571428571429</v>
       </c>
-      <c r="P29" t="n">
+      <c r="Q29" t="n">
         <v>-0.0519034249085875</v>
       </c>
-      <c r="Q29" t="n">
+      <c r="R29" t="n">
         <v>-0.131476027504787</v>
       </c>
-      <c r="R29" t="n">
+      <c r="S29" t="n">
         <v>7.0</v>
       </c>
-      <c r="S29" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T29" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="U29" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V29" t="n">
         <v>0.476161033758996</v>
       </c>
-      <c r="V29" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X29" t="n">
         <v>0.384615384615385</v>
       </c>
-      <c r="X29" t="n">
+      <c r="Y29" t="n">
         <v>0.923076923076923</v>
       </c>
     </row>
@@ -2324,33 +2414,36 @@
         <v>0.0</v>
       </c>
       <c r="O30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P30" t="n">
         <v>0.808510638297872</v>
       </c>
-      <c r="P30" t="n">
+      <c r="Q30" t="n">
         <v>0.0170972867954103</v>
       </c>
-      <c r="Q30" t="n">
+      <c r="R30" t="n">
         <v>-0.564051249164746</v>
       </c>
-      <c r="R30" t="n">
+      <c r="S30" t="n">
         <v>12.0</v>
       </c>
-      <c r="S30" t="n">
+      <c r="T30" t="n">
         <v>6.0</v>
       </c>
-      <c r="T30" t="n">
+      <c r="U30" t="n">
         <v>2.1063829787234</v>
       </c>
-      <c r="U30" t="n">
+      <c r="V30" t="n">
         <v>0.220110179249283</v>
       </c>
-      <c r="V30" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X30" t="n">
         <v>-0.473684210526316</v>
       </c>
-      <c r="X30" t="n">
+      <c r="Y30" t="n">
         <v>-0.631578947368421</v>
       </c>
     </row>
@@ -2398,33 +2491,36 @@
         <v>13.0</v>
       </c>
       <c r="O31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P31" t="n">
         <v>0.918918918918919</v>
       </c>
-      <c r="P31" t="e">
+      <c r="Q31" t="e">
         <v>#N/A</v>
       </c>
-      <c r="Q31" t="n">
+      <c r="R31" t="n">
         <v>-0.0492952851633179</v>
       </c>
-      <c r="R31" t="n">
+      <c r="S31" t="n">
         <v>12.0</v>
       </c>
-      <c r="S31" t="n">
+      <c r="T31" t="n">
         <v>5.0</v>
       </c>
-      <c r="T31" t="n">
+      <c r="U31" t="n">
         <v>2.24324324324324</v>
       </c>
-      <c r="U31" t="n">
+      <c r="V31" t="n">
         <v>0.462122069750468</v>
       </c>
-      <c r="V31" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W31" t="n">
         <v>0.0</v>
       </c>
       <c r="X31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y31" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2472,33 +2568,36 @@
         <v>14.0</v>
       </c>
       <c r="O32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P32" t="n">
         <v>0.904761904761905</v>
       </c>
-      <c r="P32" t="n">
+      <c r="Q32" t="n">
         <v>-0.47489129060507</v>
       </c>
-      <c r="Q32" t="n">
+      <c r="R32" t="n">
         <v>-0.526572999389126</v>
       </c>
-      <c r="R32" t="n">
+      <c r="S32" t="n">
         <v>12.0</v>
       </c>
-      <c r="S32" t="n">
+      <c r="T32" t="n">
         <v>5.0</v>
       </c>
-      <c r="T32" t="n">
+      <c r="U32" t="n">
         <v>2.30952380952381</v>
       </c>
-      <c r="U32" t="n">
+      <c r="V32" t="n">
         <v>0.27042766207476</v>
       </c>
-      <c r="V32" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W32" t="n">
         <v>0.0</v>
       </c>
       <c r="X32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y32" t="n">
         <v>0.105263157894737</v>
       </c>
     </row>
@@ -2546,33 +2645,36 @@
         <v>3.0</v>
       </c>
       <c r="O33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P33" t="n">
         <v>0.5</v>
       </c>
-      <c r="P33" t="n">
+      <c r="Q33" t="n">
         <v>-0.826976769629957</v>
       </c>
-      <c r="Q33" t="n">
+      <c r="R33" t="n">
         <v>-1.0</v>
       </c>
-      <c r="R33" t="n">
+      <c r="S33" t="n">
         <v>6.0</v>
       </c>
-      <c r="S33" t="n">
-        <v>2.0</v>
-      </c>
       <c r="T33" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="U33" t="n">
         <v>2.875</v>
       </c>
-      <c r="U33" t="n">
-        <v>1.0</v>
-      </c>
       <c r="V33" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X33" t="n">
         <v>-0.285714285714286</v>
       </c>
-      <c r="X33" t="n">
+      <c r="Y33" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -2620,33 +2722,36 @@
         <v>0.0</v>
       </c>
       <c r="O34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P34" t="n">
         <v>0.285714285714286</v>
       </c>
-      <c r="P34" t="n">
+      <c r="Q34" t="n">
         <v>-0.645497224367902</v>
       </c>
-      <c r="Q34" t="e">
+      <c r="R34" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R34" t="n">
+      <c r="S34" t="n">
         <v>8.0</v>
       </c>
-      <c r="S34" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T34" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="U34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V34" t="n">
         <v>0.48344537815126</v>
       </c>
-      <c r="V34" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X34" t="n">
         <v>-0.428571428571429</v>
       </c>
-      <c r="X34" t="n">
+      <c r="Y34" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -2694,33 +2799,36 @@
         <v>10.0</v>
       </c>
       <c r="O35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P35" t="n">
         <v>0.857142857142857</v>
       </c>
-      <c r="P35" t="n">
+      <c r="Q35" t="n">
         <v>-0.139202850903581</v>
       </c>
-      <c r="Q35" t="n">
+      <c r="R35" t="n">
         <v>0.0133754580519715</v>
       </c>
-      <c r="R35" t="n">
+      <c r="S35" t="n">
         <v>8.0</v>
       </c>
-      <c r="S35" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T35" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U35" t="n">
         <v>1.97619047619048</v>
       </c>
-      <c r="U35" t="n">
+      <c r="V35" t="n">
         <v>0.387365338713301</v>
       </c>
-      <c r="V35" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X35" t="n">
         <v>-0.461538461538462</v>
       </c>
-      <c r="X35" t="n">
+      <c r="Y35" t="n">
         <v>-1.15384615384615</v>
       </c>
     </row>
@@ -2768,33 +2876,36 @@
         <v>5.0</v>
       </c>
       <c r="O36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P36" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="P36" t="n">
+      <c r="Q36" t="n">
         <v>0.0910695581716403</v>
       </c>
-      <c r="Q36" t="n">
+      <c r="R36" t="n">
         <v>-0.323087514721127</v>
       </c>
-      <c r="R36" t="n">
+      <c r="S36" t="n">
         <v>10.0</v>
       </c>
-      <c r="S36" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T36" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U36" t="n">
         <v>2.16666666666667</v>
       </c>
-      <c r="U36" t="n">
+      <c r="V36" t="n">
         <v>0.728590568552368</v>
       </c>
-      <c r="V36" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X36" t="n">
         <v>-0.125</v>
       </c>
-      <c r="X36" t="n">
+      <c r="Y36" t="n">
         <v>-0.5625</v>
       </c>
     </row>
@@ -2842,33 +2953,36 @@
         <v>4.0</v>
       </c>
       <c r="O37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P37" t="n">
         <v>0.545454545454545</v>
       </c>
-      <c r="P37" t="n">
+      <c r="Q37" t="n">
         <v>0.375053278397655</v>
       </c>
-      <c r="Q37" t="n">
+      <c r="R37" t="n">
         <v>-0.113122814366088</v>
       </c>
-      <c r="R37" t="n">
+      <c r="S37" t="n">
         <v>10.0</v>
       </c>
-      <c r="S37" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T37" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U37" t="n">
         <v>2.09090909090909</v>
       </c>
-      <c r="U37" t="n">
+      <c r="V37" t="n">
         <v>0.599666326660716</v>
       </c>
-      <c r="V37" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X37" t="n">
         <v>-0.0833333333333333</v>
       </c>
-      <c r="X37" t="n">
+      <c r="Y37" t="n">
         <v>-0.25</v>
       </c>
     </row>
@@ -2916,33 +3030,36 @@
         <v>0.0</v>
       </c>
       <c r="O38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P38" t="n">
         <v>0.705882352941177</v>
       </c>
-      <c r="P38" t="n">
+      <c r="Q38" t="n">
         <v>-0.6985354731357</v>
       </c>
-      <c r="Q38" t="n">
+      <c r="R38" t="n">
         <v>-0.674086301557899</v>
       </c>
-      <c r="R38" t="n">
+      <c r="S38" t="n">
         <v>8.0</v>
       </c>
-      <c r="S38" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T38" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U38" t="n">
         <v>2.05882352941176</v>
       </c>
-      <c r="U38" t="n">
+      <c r="V38" t="n">
         <v>0.571743048085759</v>
       </c>
-      <c r="V38" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X38" t="n">
         <v>-0.181818181818182</v>
       </c>
-      <c r="X38" t="n">
+      <c r="Y38" t="n">
         <v>-0.636363636363636</v>
       </c>
     </row>
@@ -2990,33 +3107,36 @@
         <v>0.0</v>
       </c>
       <c r="O39" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P39" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q39" t="n">
         <v>-0.804469273743016</v>
       </c>
-      <c r="Q39" t="n">
+      <c r="R39" t="n">
         <v>-0.659090909090909</v>
       </c>
-      <c r="R39" t="n">
+      <c r="S39" t="n">
         <v>9.0</v>
       </c>
-      <c r="S39" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T39" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U39" t="n">
         <v>2.05882352941176</v>
       </c>
-      <c r="U39" t="n">
+      <c r="V39" t="n">
         <v>0.475535192147034</v>
       </c>
-      <c r="V39" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W39" t="n">
         <v>0.0</v>
       </c>
       <c r="X39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y39" t="n">
         <v>0.0555555555555556</v>
       </c>
     </row>
@@ -3064,33 +3184,36 @@
         <v>2.0</v>
       </c>
       <c r="O40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P40" t="n">
         <v>0.857142857142857</v>
       </c>
-      <c r="P40" t="n">
+      <c r="Q40" t="n">
         <v>0.316081465862806</v>
       </c>
-      <c r="Q40" t="n">
+      <c r="R40" t="n">
         <v>-0.156821299347095</v>
       </c>
-      <c r="R40" t="n">
+      <c r="S40" t="n">
         <v>11.0</v>
       </c>
-      <c r="S40" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T40" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U40" t="n">
         <v>2.07142857142857</v>
       </c>
-      <c r="U40" t="n">
+      <c r="V40" t="n">
         <v>0.577477211683214</v>
       </c>
-      <c r="V40" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X40" t="n">
         <v>-0.25</v>
       </c>
-      <c r="X40" t="n">
+      <c r="Y40" t="n">
         <v>-0.5</v>
       </c>
     </row>
@@ -3138,33 +3261,36 @@
         <v>9.0</v>
       </c>
       <c r="O41" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="P41" t="n">
         <v>0.784313725490196</v>
       </c>
-      <c r="P41" t="n">
+      <c r="Q41" t="n">
         <v>-0.179414079931538</v>
       </c>
-      <c r="Q41" t="n">
+      <c r="R41" t="n">
         <v>-0.141114379412457</v>
       </c>
-      <c r="R41" t="n">
+      <c r="S41" t="n">
         <v>10.0</v>
       </c>
-      <c r="S41" t="n">
+      <c r="T41" t="n">
         <v>5.0</v>
       </c>
-      <c r="T41" t="n">
+      <c r="U41" t="n">
         <v>2.05882352941176</v>
       </c>
-      <c r="U41" t="n">
+      <c r="V41" t="n">
         <v>0.359553247047997</v>
       </c>
-      <c r="V41" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X41" t="n">
         <v>-0.4375</v>
       </c>
-      <c r="X41" t="n">
+      <c r="Y41" t="n">
         <v>-0.75</v>
       </c>
     </row>
@@ -3212,33 +3338,36 @@
         <v>6.0</v>
       </c>
       <c r="O42" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="P42" t="n">
         <v>0.923076923076923</v>
       </c>
-      <c r="P42" t="n">
+      <c r="Q42" t="n">
         <v>0.105876963705021</v>
       </c>
-      <c r="Q42" t="n">
+      <c r="R42" t="n">
         <v>-0.264224300947295</v>
       </c>
-      <c r="R42" t="n">
+      <c r="S42" t="n">
         <v>6.0</v>
       </c>
-      <c r="S42" t="n">
-        <v>3.0</v>
-      </c>
       <c r="T42" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U42" t="n">
         <v>2.15384615384615</v>
       </c>
-      <c r="U42" t="n">
+      <c r="V42" t="n">
         <v>0.30785286142429</v>
       </c>
-      <c r="V42" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W42" t="n">
         <v>0.0</v>
       </c>
       <c r="X42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y42" t="n">
         <v>0.222222222222222</v>
       </c>
     </row>
@@ -3286,33 +3415,36 @@
         <v>4.0</v>
       </c>
       <c r="O43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P43" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="P43" t="n">
+      <c r="Q43" t="n">
         <v>0.063245553203368</v>
       </c>
-      <c r="Q43" t="n">
+      <c r="R43" t="n">
         <v>-0.41304347826087</v>
       </c>
-      <c r="R43" t="n">
+      <c r="S43" t="n">
         <v>6.0</v>
       </c>
-      <c r="S43" t="n">
-        <v>3.0</v>
-      </c>
       <c r="T43" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U43" t="n">
         <v>1.83333333333333</v>
       </c>
-      <c r="U43" t="n">
+      <c r="V43" t="n">
         <v>0.529047619047619</v>
       </c>
-      <c r="V43" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X43" t="n">
         <v>0.142857142857143</v>
       </c>
-      <c r="X43" t="n">
+      <c r="Y43" t="n">
         <v>0.142857142857143</v>
       </c>
     </row>
@@ -3360,33 +3492,36 @@
         <v>13.0</v>
       </c>
       <c r="O44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P44" t="n">
         <v>0.645161290322581</v>
       </c>
-      <c r="P44" t="n">
+      <c r="Q44" t="n">
         <v>0.144353442649549</v>
       </c>
-      <c r="Q44" t="n">
+      <c r="R44" t="n">
         <v>-0.10744675350062</v>
       </c>
-      <c r="R44" t="n">
+      <c r="S44" t="n">
         <v>12.0</v>
       </c>
-      <c r="S44" t="n">
+      <c r="T44" t="n">
         <v>5.0</v>
       </c>
-      <c r="T44" t="n">
+      <c r="U44" t="n">
         <v>2.25806451612903</v>
       </c>
-      <c r="U44" t="n">
+      <c r="V44" t="n">
         <v>0.481905511435627</v>
       </c>
-      <c r="V44" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X44" t="n">
         <v>0.1</v>
       </c>
-      <c r="X44" t="n">
+      <c r="Y44" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -3434,33 +3569,36 @@
         <v>0.0</v>
       </c>
       <c r="O45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P45" t="n">
         <v>0.133333333333333</v>
       </c>
-      <c r="P45" t="n">
+      <c r="Q45" t="n">
         <v>0.307863137153618</v>
       </c>
-      <c r="Q45" t="n">
+      <c r="R45" t="n">
         <v>-0.440254653042281</v>
       </c>
-      <c r="R45" t="n">
+      <c r="S45" t="n">
         <v>10.0</v>
       </c>
-      <c r="S45" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T45" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U45" t="n">
         <v>2.13333333333333</v>
       </c>
-      <c r="U45" t="n">
+      <c r="V45" t="n">
         <v>0.365871138618564</v>
       </c>
-      <c r="V45" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X45" t="n">
         <v>-0.1</v>
       </c>
-      <c r="X45" t="n">
+      <c r="Y45" t="n">
         <v>-0.4</v>
       </c>
     </row>
@@ -3508,33 +3646,36 @@
         <v>12.0</v>
       </c>
       <c r="O46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P46" t="n">
         <v>0.588235294117647</v>
       </c>
-      <c r="P46" t="n">
+      <c r="Q46" t="n">
         <v>-0.525923706140778</v>
       </c>
-      <c r="Q46" t="n">
+      <c r="R46" t="n">
         <v>-0.681681697630259</v>
       </c>
-      <c r="R46" t="n">
-        <v>4.0</v>
-      </c>
       <c r="S46" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="T46" t="n">
         <v>2.0</v>
       </c>
       <c r="U46" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V46" t="n">
         <v>0.975308641975309</v>
       </c>
-      <c r="V46" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X46" t="n">
         <v>-0.636363636363636</v>
       </c>
-      <c r="X46" t="n">
+      <c r="Y46" t="n">
         <v>-2.0</v>
       </c>
     </row>
@@ -3582,33 +3723,36 @@
         <v>2.0</v>
       </c>
       <c r="O47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P47" t="n">
         <v>0.733333333333333</v>
       </c>
-      <c r="P47" t="n">
+      <c r="Q47" t="n">
         <v>-0.634337844326788</v>
       </c>
-      <c r="Q47" t="n">
+      <c r="R47" t="n">
         <v>-0.0671196063665116</v>
       </c>
-      <c r="R47" t="n">
+      <c r="S47" t="n">
         <v>11.0</v>
       </c>
-      <c r="S47" t="n">
+      <c r="T47" t="n">
         <v>5.0</v>
       </c>
-      <c r="T47" t="n">
+      <c r="U47" t="n">
         <v>2.06666666666667</v>
       </c>
-      <c r="U47" t="n">
+      <c r="V47" t="n">
         <v>0.366651554481318</v>
       </c>
-      <c r="V47" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X47" t="n">
         <v>-0.461538461538462</v>
       </c>
-      <c r="X47" t="n">
+      <c r="Y47" t="n">
         <v>-1.46153846153846</v>
       </c>
     </row>
@@ -3656,33 +3800,36 @@
         <v>3.0</v>
       </c>
       <c r="O48" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="P48" t="n">
         <v>0.133333333333333</v>
       </c>
-      <c r="P48" t="n">
+      <c r="Q48" t="n">
         <v>0.0496291666985473</v>
       </c>
-      <c r="Q48" t="n">
+      <c r="R48" t="n">
         <v>-0.228468383365844</v>
       </c>
-      <c r="R48" t="n">
+      <c r="S48" t="n">
         <v>10.0</v>
       </c>
-      <c r="S48" t="n">
+      <c r="T48" t="n">
         <v>5.0</v>
       </c>
-      <c r="T48" t="n">
-        <v>2.0</v>
-      </c>
       <c r="U48" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V48" t="n">
         <v>0.405575376689064</v>
       </c>
-      <c r="V48" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X48" t="n">
         <v>0.466666666666667</v>
       </c>
-      <c r="X48" t="n">
+      <c r="Y48" t="n">
         <v>1.13333333333333</v>
       </c>
     </row>
@@ -3730,33 +3877,36 @@
         <v>0.0</v>
       </c>
       <c r="O49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P49" t="n">
         <v>0.444444444444444</v>
       </c>
-      <c r="P49" t="n">
+      <c r="Q49" t="n">
         <v>-0.602010055881586</v>
       </c>
-      <c r="Q49" t="n">
+      <c r="R49" t="n">
         <v>-0.55501199749894</v>
       </c>
-      <c r="R49" t="n">
+      <c r="S49" t="n">
         <v>8.0</v>
       </c>
-      <c r="S49" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T49" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="U49" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V49" t="n">
         <v>0.444122771836007</v>
       </c>
-      <c r="V49" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X49" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="X49" t="n">
+      <c r="Y49" t="n">
         <v>0.166666666666667</v>
       </c>
     </row>
@@ -3804,33 +3954,36 @@
         <v>5.0</v>
       </c>
       <c r="O50" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P50" t="n">
         <v>0.782608695652174</v>
       </c>
-      <c r="P50" t="n">
+      <c r="Q50" t="n">
         <v>-0.453825519709041</v>
       </c>
-      <c r="Q50" t="n">
+      <c r="R50" t="n">
         <v>-0.592853696825125</v>
       </c>
-      <c r="R50" t="n">
+      <c r="S50" t="n">
         <v>6.0</v>
       </c>
-      <c r="S50" t="n">
-        <v>3.0</v>
-      </c>
       <c r="T50" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="U50" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V50" t="n">
         <v>0.813373110186836</v>
       </c>
-      <c r="V50" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X50" t="n">
         <v>0.363636363636364</v>
       </c>
-      <c r="X50" t="n">
+      <c r="Y50" t="n">
         <v>0.727272727272727</v>
       </c>
     </row>
@@ -3878,33 +4031,36 @@
         <v>4.0</v>
       </c>
       <c r="O51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P51" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="P51" t="n">
+      <c r="Q51" t="n">
         <v>0.334021328561343</v>
       </c>
-      <c r="Q51" t="n">
+      <c r="R51" t="n">
         <v>-0.79692031510165</v>
       </c>
-      <c r="R51" t="n">
+      <c r="S51" t="n">
         <v>8.0</v>
       </c>
-      <c r="S51" t="n">
-        <v>3.0</v>
-      </c>
       <c r="T51" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U51" t="n">
         <v>2.13333333333333</v>
       </c>
-      <c r="U51" t="n">
+      <c r="V51" t="n">
         <v>0.879274223718668</v>
       </c>
-      <c r="V51" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X51" t="n">
         <v>-0.363636363636364</v>
       </c>
-      <c r="X51" t="n">
+      <c r="Y51" t="n">
         <v>-1.09090909090909</v>
       </c>
     </row>
@@ -3952,33 +4108,36 @@
         <v>20.0</v>
       </c>
       <c r="O52" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="P52" t="n">
         <v>0.986666666666667</v>
       </c>
-      <c r="P52" t="n">
+      <c r="Q52" t="n">
         <v>-0.188946015424164</v>
       </c>
-      <c r="Q52" t="n">
+      <c r="R52" t="n">
         <v>-0.33148511509831</v>
       </c>
-      <c r="R52" t="n">
+      <c r="S52" t="n">
         <v>6.0</v>
       </c>
-      <c r="S52" t="n">
-        <v>3.0</v>
-      </c>
       <c r="T52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U52" t="n">
         <v>2.10666666666667</v>
       </c>
-      <c r="U52" t="n">
+      <c r="V52" t="n">
         <v>0.408921309726237</v>
       </c>
-      <c r="V52" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W52" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X52" t="n">
         <v>-0.1875</v>
       </c>
-      <c r="X52" t="n">
+      <c r="Y52" t="n">
         <v>-0.5625</v>
       </c>
     </row>
@@ -4026,33 +4185,36 @@
         <v>0.0</v>
       </c>
       <c r="O53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P53" t="n">
         <v>0.96551724137931</v>
       </c>
-      <c r="P53" t="n">
+      <c r="Q53" t="n">
         <v>-0.115384615384615</v>
       </c>
-      <c r="Q53" t="n">
+      <c r="R53" t="n">
         <v>-0.234666992909049</v>
       </c>
-      <c r="R53" t="n">
+      <c r="S53" t="n">
         <v>12.0</v>
       </c>
-      <c r="S53" t="n">
+      <c r="T53" t="n">
         <v>6.0</v>
       </c>
-      <c r="T53" t="n">
-        <v>2.0</v>
-      </c>
       <c r="U53" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V53" t="n">
         <v>0.213107810896417</v>
       </c>
-      <c r="V53" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X53" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="X53" t="n">
+      <c r="Y53" t="n">
         <v>0.166666666666667</v>
       </c>
     </row>
@@ -4100,33 +4262,36 @@
         <v>2.0</v>
       </c>
       <c r="O54" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="P54" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q54" t="n">
         <v>-0.423728813559321</v>
       </c>
-      <c r="Q54" t="n">
+      <c r="R54" t="n">
         <v>-0.448275862068965</v>
       </c>
-      <c r="R54" t="n">
+      <c r="S54" t="n">
         <v>9.0</v>
       </c>
-      <c r="S54" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T54" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U54" t="n">
         <v>2.16666666666667</v>
       </c>
-      <c r="U54" t="n">
+      <c r="V54" t="n">
         <v>0.48344537815126</v>
       </c>
-      <c r="V54" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X54" t="n">
         <v>0.285714285714286</v>
       </c>
-      <c r="X54" t="n">
+      <c r="Y54" t="n">
         <v>0.571428571428571</v>
       </c>
     </row>
@@ -4174,33 +4339,36 @@
         <v>6.0</v>
       </c>
       <c r="O55" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P55" t="n">
         <v>0.777777777777778</v>
       </c>
-      <c r="P55" t="n">
+      <c r="Q55" t="n">
         <v>-0.655172413793103</v>
       </c>
-      <c r="Q55" t="n">
+      <c r="R55" t="n">
         <v>-0.466705410395215</v>
       </c>
-      <c r="R55" t="n">
+      <c r="S55" t="n">
         <v>12.0</v>
       </c>
-      <c r="S55" t="n">
+      <c r="T55" t="n">
         <v>5.0</v>
       </c>
-      <c r="T55" t="n">
+      <c r="U55" t="n">
         <v>2.22222222222222</v>
       </c>
-      <c r="U55" t="n">
+      <c r="V55" t="n">
         <v>0.382370605159211</v>
       </c>
-      <c r="V55" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X55" t="n">
         <v>0.25</v>
       </c>
-      <c r="X55" t="n">
+      <c r="Y55" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -4248,33 +4416,36 @@
         <v>6.0</v>
       </c>
       <c r="O56" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="P56" t="n">
         <v>0.181818181818182</v>
       </c>
-      <c r="P56" t="n">
+      <c r="Q56" t="n">
         <v>-0.119024633360947</v>
       </c>
-      <c r="Q56" t="n">
+      <c r="R56" t="n">
         <v>-0.0152728381860816</v>
       </c>
-      <c r="R56" t="n">
+      <c r="S56" t="n">
         <v>10.0</v>
       </c>
-      <c r="S56" t="n">
+      <c r="T56" t="n">
         <v>5.0</v>
       </c>
-      <c r="T56" t="n">
+      <c r="U56" t="n">
         <v>2.24242424242424</v>
       </c>
-      <c r="U56" t="n">
+      <c r="V56" t="n">
         <v>0.309847290241654</v>
       </c>
-      <c r="V56" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X56" t="n">
         <v>-0.333333333333333</v>
       </c>
-      <c r="X56" t="n">
+      <c r="Y56" t="n">
         <v>-0.722222222222222</v>
       </c>
     </row>
@@ -4322,33 +4493,36 @@
         <v>4.0</v>
       </c>
       <c r="O57" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P57" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R57" t="n">
         <v>-0.5</v>
       </c>
-      <c r="R57" t="n">
+      <c r="S57" t="n">
         <v>10.0</v>
       </c>
-      <c r="S57" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T57" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U57" t="n">
         <v>2.33333333333333</v>
       </c>
-      <c r="U57" t="n">
+      <c r="V57" t="n">
         <v>0.636538461538461</v>
       </c>
-      <c r="V57" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X57" t="n">
         <v>0.142857142857143</v>
       </c>
-      <c r="X57" t="n">
+      <c r="Y57" t="n">
         <v>0.714285714285714</v>
       </c>
     </row>
@@ -4396,33 +4570,36 @@
         <v>15.0</v>
       </c>
       <c r="O58" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P58" t="n">
         <v>0.476190476190476</v>
       </c>
-      <c r="P58" t="n">
+      <c r="Q58" t="n">
         <v>0.401434373063499</v>
       </c>
-      <c r="Q58" t="n">
+      <c r="R58" t="n">
         <v>-0.285231022581493</v>
       </c>
-      <c r="R58" t="n">
+      <c r="S58" t="n">
         <v>11.0</v>
       </c>
-      <c r="S58" t="n">
+      <c r="T58" t="n">
         <v>5.0</v>
       </c>
-      <c r="T58" t="n">
+      <c r="U58" t="n">
         <v>2.14285714285714</v>
       </c>
-      <c r="U58" t="n">
+      <c r="V58" t="n">
         <v>0.262058407677909</v>
       </c>
-      <c r="V58" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X58" t="n">
         <v>-0.230769230769231</v>
       </c>
-      <c r="X58" t="n">
+      <c r="Y58" t="n">
         <v>-0.230769230769231</v>
       </c>
     </row>
@@ -4473,30 +4650,33 @@
         <v>0.0</v>
       </c>
       <c r="P59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q59" t="n">
         <v>-0.0542113592649565</v>
       </c>
-      <c r="Q59" t="n">
+      <c r="R59" t="n">
         <v>0.071743005397944</v>
       </c>
-      <c r="R59" t="n">
+      <c r="S59" t="n">
         <v>16.0</v>
       </c>
-      <c r="S59" t="n">
+      <c r="T59" t="n">
         <v>8.0</v>
       </c>
-      <c r="T59" t="n">
-        <v>2.0</v>
-      </c>
       <c r="U59" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V59" t="n">
         <v>0.278606575420173</v>
       </c>
-      <c r="V59" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W59" t="n">
         <v>0.0</v>
       </c>
       <c r="X59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y59" t="n">
         <v>-0.3</v>
       </c>
     </row>
@@ -4544,33 +4724,36 @@
         <v>5.0</v>
       </c>
       <c r="O60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P60" t="n">
         <v>0.952380952380952</v>
       </c>
-      <c r="P60" t="n">
+      <c r="Q60" t="n">
         <v>0.447368421052632</v>
       </c>
-      <c r="Q60" t="n">
+      <c r="R60" t="n">
         <v>-0.674755865713626</v>
       </c>
-      <c r="R60" t="n">
+      <c r="S60" t="n">
         <v>8.0</v>
       </c>
-      <c r="S60" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T60" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="U60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V60" t="n">
         <v>0.553365384615385</v>
       </c>
-      <c r="V60" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X60" t="n">
         <v>0.25</v>
       </c>
-      <c r="X60" t="n">
+      <c r="Y60" t="n">
         <v>0.416666666666667</v>
       </c>
     </row>
@@ -4618,33 +4801,36 @@
         <v>6.0</v>
       </c>
       <c r="O61" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="P61" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q61" t="n">
         <v>0.181818181818181</v>
       </c>
-      <c r="Q61" t="n">
+      <c r="R61" t="n">
         <v>-0.551020408163265</v>
       </c>
-      <c r="R61" t="n">
+      <c r="S61" t="n">
         <v>8.0</v>
       </c>
-      <c r="S61" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T61" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="U61" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V61" t="n">
         <v>0.716931818181818</v>
       </c>
-      <c r="V61" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X61" t="n">
         <v>-0.0833333333333333</v>
       </c>
-      <c r="X61" t="n">
+      <c r="Y61" t="n">
         <v>-0.25</v>
       </c>
     </row>
@@ -4692,33 +4878,36 @@
         <v>18.0</v>
       </c>
       <c r="O62" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="P62" t="n">
         <v>0.72</v>
       </c>
-      <c r="P62" t="n">
+      <c r="Q62" t="n">
         <v>0.266996858318825</v>
       </c>
-      <c r="Q62" t="n">
+      <c r="R62" t="n">
         <v>-0.134510084705172</v>
       </c>
-      <c r="R62" t="n">
+      <c r="S62" t="n">
         <v>14.0</v>
       </c>
-      <c r="S62" t="n">
+      <c r="T62" t="n">
         <v>5.0</v>
       </c>
-      <c r="T62" t="n">
+      <c r="U62" t="n">
         <v>2.64</v>
       </c>
-      <c r="U62" t="n">
+      <c r="V62" t="n">
         <v>0.416329187691765</v>
       </c>
-      <c r="V62" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W62" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X62" t="n">
         <v>-0.3125</v>
       </c>
-      <c r="X62" t="n">
+      <c r="Y62" t="n">
         <v>-0.9375</v>
       </c>
     </row>
@@ -4766,33 +4955,36 @@
         <v>0.0</v>
       </c>
       <c r="O63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P63" t="n">
         <v>0.470588235294118</v>
       </c>
-      <c r="P63" t="e">
+      <c r="Q63" t="e">
         <v>#N/A</v>
       </c>
-      <c r="Q63" t="n">
+      <c r="R63" t="n">
         <v>-0.319857179551711</v>
       </c>
-      <c r="R63" t="n">
+      <c r="S63" t="n">
         <v>12.0</v>
       </c>
-      <c r="S63" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T63" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U63" t="n">
         <v>2.52941176470588</v>
       </c>
-      <c r="U63" t="n">
+      <c r="V63" t="n">
         <v>0.620016129032258</v>
       </c>
-      <c r="V63" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X63" t="n">
         <v>-0.833333333333333</v>
       </c>
-      <c r="X63" t="n">
+      <c r="Y63" t="n">
         <v>-1.66666666666667</v>
       </c>
     </row>
@@ -4840,33 +5032,36 @@
         <v>0.0</v>
       </c>
       <c r="O64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P64" t="n">
         <v>0.745762711864407</v>
       </c>
-      <c r="P64" t="n">
+      <c r="Q64" t="n">
         <v>-0.0772182181531277</v>
       </c>
-      <c r="Q64" t="n">
+      <c r="R64" t="n">
         <v>-0.0361173327754251</v>
       </c>
-      <c r="R64" t="n">
+      <c r="S64" t="n">
         <v>17.0</v>
       </c>
-      <c r="S64" t="n">
+      <c r="T64" t="n">
         <v>8.0</v>
       </c>
-      <c r="T64" t="n">
+      <c r="U64" t="n">
         <v>2.03389830508475</v>
       </c>
-      <c r="U64" t="n">
+      <c r="V64" t="n">
         <v>0.338936736350951</v>
       </c>
-      <c r="V64" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X64" t="n">
         <v>-0.411764705882353</v>
       </c>
-      <c r="X64" t="n">
+      <c r="Y64" t="n">
         <v>-0.911764705882353</v>
       </c>
     </row>
@@ -4914,33 +5109,36 @@
         <v>2.0</v>
       </c>
       <c r="O65" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P65" t="n">
         <v>0.727272727272727</v>
       </c>
-      <c r="P65" t="n">
+      <c r="Q65" t="n">
         <v>0.220433357088703</v>
       </c>
-      <c r="Q65" t="n">
+      <c r="R65" t="n">
         <v>-0.572660366596452</v>
       </c>
-      <c r="R65" t="n">
+      <c r="S65" t="n">
         <v>12.0</v>
       </c>
-      <c r="S65" t="n">
+      <c r="T65" t="n">
         <v>6.0</v>
       </c>
-      <c r="T65" t="n">
-        <v>2.0</v>
-      </c>
       <c r="U65" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V65" t="n">
         <v>0.417154476113807</v>
       </c>
-      <c r="V65" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W65" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X65" t="n">
         <v>0.157894736842105</v>
       </c>
-      <c r="X65" t="n">
+      <c r="Y65" t="n">
         <v>0.526315789473684</v>
       </c>
     </row>
@@ -4988,33 +5186,36 @@
         <v>0.0</v>
       </c>
       <c r="O66" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P66" t="n">
         <v>0.4</v>
       </c>
-      <c r="P66" t="n">
+      <c r="Q66" t="n">
         <v>-0.111111111111113</v>
       </c>
-      <c r="Q66" t="n">
+      <c r="R66" t="n">
         <v>-0.514791561670229</v>
       </c>
-      <c r="R66" t="n">
+      <c r="S66" t="n">
         <v>11.0</v>
       </c>
-      <c r="S66" t="n">
+      <c r="T66" t="n">
         <v>5.0</v>
       </c>
-      <c r="T66" t="n">
+      <c r="U66" t="n">
         <v>2.2</v>
       </c>
-      <c r="U66" t="n">
+      <c r="V66" t="n">
         <v>0.389825495415558</v>
       </c>
-      <c r="V66" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W66" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X66" t="n">
         <v>-0.555555555555556</v>
       </c>
-      <c r="X66" t="n">
+      <c r="Y66" t="n">
         <v>-1.44444444444444</v>
       </c>
     </row>
@@ -5062,33 +5263,36 @@
         <v>20.0</v>
       </c>
       <c r="O67" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="P67" t="n">
         <v>0.6875</v>
       </c>
-      <c r="P67" t="n">
+      <c r="Q67" t="n">
         <v>0.391713100928669</v>
       </c>
-      <c r="Q67" t="n">
+      <c r="R67" t="n">
         <v>-0.365123550098154</v>
       </c>
-      <c r="R67" t="n">
+      <c r="S67" t="n">
         <v>12.0</v>
       </c>
-      <c r="S67" t="n">
+      <c r="T67" t="n">
         <v>5.0</v>
       </c>
-      <c r="T67" t="n">
+      <c r="U67" t="n">
         <v>2.28125</v>
       </c>
-      <c r="U67" t="n">
+      <c r="V67" t="n">
         <v>0.513697362471116</v>
       </c>
-      <c r="V67" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W67" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X67" t="n">
         <v>-0.473684210526316</v>
       </c>
-      <c r="X67" t="n">
+      <c r="Y67" t="n">
         <v>-1.10526315789474</v>
       </c>
     </row>
@@ -5136,33 +5340,36 @@
         <v>6.0</v>
       </c>
       <c r="O68" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P68" t="n">
         <v>0.9</v>
       </c>
-      <c r="P68" t="n">
+      <c r="Q68" t="n">
         <v>-0.438848920863309</v>
       </c>
-      <c r="Q68" t="n">
+      <c r="R68" t="n">
         <v>-0.615010337180622</v>
       </c>
-      <c r="R68" t="n">
+      <c r="S68" t="n">
         <v>5.0</v>
       </c>
-      <c r="S68" t="n">
-        <v>2.0</v>
-      </c>
       <c r="T68" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="U68" t="n">
         <v>1.6</v>
       </c>
-      <c r="U68" t="n">
+      <c r="V68" t="n">
         <v>0.881313131313131</v>
       </c>
-      <c r="V68" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W68" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X68" t="n">
         <v>-0.25</v>
       </c>
-      <c r="X68" t="n">
+      <c r="Y68" t="n">
         <v>-0.75</v>
       </c>
     </row>
@@ -5210,33 +5417,36 @@
         <v>6.0</v>
       </c>
       <c r="O69" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P69" t="n">
         <v>0.636363636363636</v>
       </c>
-      <c r="P69" t="n">
+      <c r="Q69" t="n">
         <v>-0.00841078887815635</v>
       </c>
-      <c r="Q69" t="n">
+      <c r="R69" t="n">
         <v>-0.0452510166166453</v>
       </c>
-      <c r="R69" t="n">
+      <c r="S69" t="n">
         <v>7.0</v>
       </c>
-      <c r="S69" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T69" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U69" t="n">
         <v>1.72727272727273</v>
       </c>
-      <c r="U69" t="n">
+      <c r="V69" t="n">
         <v>0.435480929888825</v>
       </c>
-      <c r="V69" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W69" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X69" t="n">
         <v>-0.2</v>
       </c>
-      <c r="X69" t="n">
+      <c r="Y69" t="n">
         <v>-0.3</v>
       </c>
     </row>
@@ -5284,33 +5494,36 @@
         <v>0.0</v>
       </c>
       <c r="O70" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P70" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q70" t="n">
         <v>-0.538461538461538</v>
       </c>
-      <c r="Q70" t="n">
+      <c r="R70" t="n">
         <v>-0.640378548895899</v>
       </c>
-      <c r="R70" t="n">
-        <v>3.0</v>
-      </c>
       <c r="S70" t="n">
         <v>3.0</v>
       </c>
       <c r="T70" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="U70" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V70" t="n">
         <v>0.798357500895095</v>
       </c>
-      <c r="V70" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W70" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X70" t="n">
         <v>0.222222222222222</v>
       </c>
-      <c r="X70" t="n">
+      <c r="Y70" t="n">
         <v>0.777777777777778</v>
       </c>
     </row>
@@ -5358,33 +5571,36 @@
         <v>4.0</v>
       </c>
       <c r="O71" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P71" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q71" t="n">
         <v>-0.213186813186814</v>
       </c>
-      <c r="Q71" t="n">
+      <c r="R71" t="n">
         <v>-0.688622754491018</v>
       </c>
-      <c r="R71" t="n">
+      <c r="S71" t="n">
         <v>6.0</v>
       </c>
-      <c r="S71" t="n">
-        <v>2.0</v>
-      </c>
       <c r="T71" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="U71" t="n">
         <v>2.08333333333333</v>
       </c>
-      <c r="U71" t="n">
+      <c r="V71" t="n">
         <v>0.84006734006734</v>
       </c>
-      <c r="V71" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W71" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X71" t="n">
         <v>0.375</v>
       </c>
-      <c r="X71" t="n">
+      <c r="Y71" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -5432,33 +5648,36 @@
         <v>2.0</v>
       </c>
       <c r="O72" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P72" t="n">
         <v>0.769230769230769</v>
       </c>
-      <c r="P72" t="n">
+      <c r="Q72" t="n">
         <v>-0.433012701892222</v>
       </c>
-      <c r="Q72" t="n">
+      <c r="R72" t="n">
         <v>-1.0</v>
       </c>
-      <c r="R72" t="n">
-        <v>4.0</v>
-      </c>
       <c r="S72" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="T72" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="U72" t="n">
         <v>1.23076923076923</v>
       </c>
-      <c r="U72" t="n">
-        <v>1.0</v>
-      </c>
       <c r="V72" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W72" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X72" t="n">
         <v>0.111111111111111</v>
       </c>
-      <c r="X72" t="n">
+      <c r="Y72" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -5506,33 +5725,36 @@
         <v>0.0</v>
       </c>
       <c r="O73" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P73" t="n">
         <v>0.923076923076923</v>
       </c>
-      <c r="P73" t="n">
+      <c r="Q73" t="n">
         <v>-0.462621002059225</v>
       </c>
-      <c r="Q73" t="n">
+      <c r="R73" t="n">
         <v>-0.342767155452847</v>
       </c>
-      <c r="R73" t="n">
+      <c r="S73" t="n">
         <v>9.0</v>
       </c>
-      <c r="S73" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T73" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U73" t="n">
         <v>1.53846153846154</v>
       </c>
-      <c r="U73" t="n">
+      <c r="V73" t="n">
         <v>0.604501838974489</v>
       </c>
-      <c r="V73" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W73" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X73" t="n">
         <v>-0.166666666666667</v>
       </c>
-      <c r="X73" t="n">
+      <c r="Y73" t="n">
         <v>-0.666666666666667</v>
       </c>
     </row>
@@ -5580,33 +5802,36 @@
         <v>0.0</v>
       </c>
       <c r="O74" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P74" t="n">
         <v>0.736842105263158</v>
       </c>
-      <c r="P74" t="n">
+      <c r="Q74" t="n">
         <v>-0.0555555555555572</v>
       </c>
-      <c r="Q74" t="n">
+      <c r="R74" t="n">
         <v>0.0948840144095737</v>
       </c>
-      <c r="R74" t="n">
+      <c r="S74" t="n">
         <v>8.0</v>
       </c>
-      <c r="S74" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T74" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U74" t="n">
         <v>1.84210526315789</v>
       </c>
-      <c r="U74" t="n">
+      <c r="V74" t="n">
         <v>0.622210247735458</v>
       </c>
-      <c r="V74" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W74" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X74" t="n">
         <v>-0.444444444444444</v>
       </c>
-      <c r="X74" t="n">
+      <c r="Y74" t="n">
         <v>-1.55555555555556</v>
       </c>
     </row>
@@ -5654,33 +5879,36 @@
         <v>2.0</v>
       </c>
       <c r="O75" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P75" t="n">
         <v>0.444444444444444</v>
       </c>
-      <c r="P75" t="n">
-        <v>0.0</v>
-      </c>
       <c r="Q75" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R75" t="n">
         <v>-0.8002304995806</v>
       </c>
-      <c r="R75" t="n">
-        <v>4.0</v>
-      </c>
       <c r="S75" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="T75" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U75" t="n">
         <v>1.05555555555556</v>
       </c>
-      <c r="U75" t="n">
+      <c r="V75" t="n">
         <v>0.837120619852018</v>
       </c>
-      <c r="V75" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W75" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X75" t="n">
         <v>-0.666666666666667</v>
       </c>
-      <c r="X75" t="n">
+      <c r="Y75" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -5728,33 +5956,36 @@
         <v>0.0</v>
       </c>
       <c r="O76" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P76" t="n">
         <v>0.923076923076923</v>
       </c>
-      <c r="P76" t="n">
+      <c r="Q76" t="n">
         <v>-0.241960612823267</v>
       </c>
-      <c r="Q76" t="n">
+      <c r="R76" t="n">
         <v>-0.663303589392119</v>
       </c>
-      <c r="R76" t="n">
-        <v>4.0</v>
-      </c>
       <c r="S76" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="T76" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U76" t="n">
         <v>1.07692307692308</v>
       </c>
-      <c r="U76" t="n">
+      <c r="V76" t="n">
         <v>0.885304089849544</v>
       </c>
-      <c r="V76" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W76" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X76" t="n">
         <v>0.153846153846154</v>
       </c>
-      <c r="X76" t="n">
+      <c r="Y76" t="n">
         <v>0.230769230769231</v>
       </c>
     </row>
@@ -5802,33 +6033,36 @@
         <v>6.0</v>
       </c>
       <c r="O77" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P77" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q77" t="n">
         <v>-0.229050279329611</v>
       </c>
-      <c r="Q77" t="n">
+      <c r="R77" t="n">
         <v>-0.363636363636363</v>
       </c>
-      <c r="R77" t="n">
-        <v>3.0</v>
-      </c>
       <c r="S77" t="n">
         <v>3.0</v>
       </c>
       <c r="T77" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="U77" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V77" t="n">
         <v>0.343039640098464</v>
       </c>
-      <c r="V77" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W77" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X77" t="n">
         <v>0.375</v>
       </c>
-      <c r="X77" t="n">
+      <c r="Y77" t="n">
         <v>0.625</v>
       </c>
     </row>
@@ -5876,33 +6110,36 @@
         <v>3.0</v>
       </c>
       <c r="O78" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P78" t="n">
         <v>0.695652173913043</v>
       </c>
-      <c r="P78" t="n">
+      <c r="Q78" t="n">
         <v>-0.0541984271657117</v>
       </c>
-      <c r="Q78" t="n">
+      <c r="R78" t="n">
         <v>-0.466220131089741</v>
       </c>
-      <c r="R78" t="n">
-        <v>4.0</v>
-      </c>
       <c r="S78" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="T78" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U78" t="n">
         <v>1.34782608695652</v>
       </c>
-      <c r="U78" t="n">
+      <c r="V78" t="n">
         <v>0.522624815271874</v>
       </c>
-      <c r="V78" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W78" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X78" t="n">
         <v>0.0909090909090909</v>
       </c>
-      <c r="X78" t="n">
+      <c r="Y78" t="n">
         <v>0.272727272727273</v>
       </c>
     </row>
@@ -5950,33 +6187,36 @@
         <v>4.0</v>
       </c>
       <c r="O79" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P79" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q79" t="n">
         <v>-0.415730337078652</v>
       </c>
-      <c r="Q79" t="n">
+      <c r="R79" t="n">
         <v>-0.711111111111111</v>
       </c>
-      <c r="R79" t="n">
-        <v>4.0</v>
-      </c>
       <c r="S79" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="T79" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U79" t="n">
         <v>1.14285714285714</v>
       </c>
-      <c r="U79" t="n">
+      <c r="V79" t="n">
         <v>0.478076923076923</v>
       </c>
-      <c r="V79" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W79" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X79" t="n">
         <v>-0.142857142857143</v>
       </c>
-      <c r="X79" t="n">
+      <c r="Y79" t="n">
         <v>-0.571428571428571</v>
       </c>
     </row>
@@ -6024,33 +6264,36 @@
         <v>0.0</v>
       </c>
       <c r="O80" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P80" t="n">
         <v>0.827586206896552</v>
       </c>
-      <c r="P80" t="n">
+      <c r="Q80" t="n">
         <v>-0.260869565217392</v>
       </c>
-      <c r="Q80" t="n">
+      <c r="R80" t="n">
         <v>-0.519449606963034</v>
       </c>
-      <c r="R80" t="n">
+      <c r="S80" t="n">
         <v>6.0</v>
       </c>
-      <c r="S80" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T80" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U80" t="n">
         <v>1.6551724137931</v>
       </c>
-      <c r="U80" t="n">
+      <c r="V80" t="n">
         <v>0.672220204038386</v>
       </c>
-      <c r="V80" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W80" t="n">
         <v>0.0</v>
       </c>
       <c r="X80" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y80" t="n">
         <v>-0.307692307692308</v>
       </c>
     </row>
@@ -6098,33 +6341,36 @@
         <v>7.0</v>
       </c>
       <c r="O81" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P81" t="n">
         <v>0.893617021276596</v>
       </c>
-      <c r="P81" t="n">
-        <v>0.0</v>
-      </c>
       <c r="Q81" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R81" t="n">
         <v>-0.310859309954433</v>
       </c>
-      <c r="R81" t="n">
+      <c r="S81" t="n">
         <v>9.0</v>
       </c>
-      <c r="S81" t="n">
+      <c r="T81" t="n">
         <v>5.0</v>
       </c>
-      <c r="T81" t="n">
+      <c r="U81" t="n">
         <v>1.27659574468085</v>
       </c>
-      <c r="U81" t="n">
+      <c r="V81" t="n">
         <v>0.352708028682308</v>
       </c>
-      <c r="V81" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W81" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X81" t="n">
         <v>-0.368421052631579</v>
       </c>
-      <c r="X81" t="n">
+      <c r="Y81" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -6172,33 +6418,36 @@
         <v>4.0</v>
       </c>
       <c r="O82" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P82" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q82" t="n">
         <v>-0.56</v>
       </c>
-      <c r="Q82" t="n">
+      <c r="R82" t="n">
         <v>-0.351254480286739</v>
       </c>
-      <c r="R82" t="n">
+      <c r="S82" t="n">
         <v>9.0</v>
       </c>
-      <c r="S82" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T82" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U82" t="n">
         <v>2.15384615384615</v>
       </c>
-      <c r="U82" t="n">
+      <c r="V82" t="n">
         <v>0.543288582756728</v>
       </c>
-      <c r="V82" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W82" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X82" t="n">
         <v>-0.25</v>
       </c>
-      <c r="X82" t="n">
+      <c r="Y82" t="n">
         <v>-0.5</v>
       </c>
     </row>
@@ -6246,33 +6495,36 @@
         <v>1.0</v>
       </c>
       <c r="O83" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P83" t="n">
         <v>0.8</v>
       </c>
-      <c r="P83" t="n">
+      <c r="Q83" t="n">
         <v>-0.53452248382485</v>
       </c>
-      <c r="Q83" t="n">
+      <c r="R83" t="n">
         <v>-1.0</v>
       </c>
-      <c r="R83" t="n">
+      <c r="S83" t="n">
         <v>6.0</v>
       </c>
-      <c r="S83" t="n">
-        <v>2.0</v>
-      </c>
       <c r="T83" t="n">
         <v>2.0</v>
       </c>
       <c r="U83" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="V83" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W83" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X83" t="n">
         <v>0.142857142857143</v>
       </c>
-      <c r="X83" t="n">
+      <c r="Y83" t="n">
         <v>0.142857142857143</v>
       </c>
     </row>
@@ -6320,33 +6572,36 @@
         <v>0.0</v>
       </c>
       <c r="O84" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P84" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q84" t="n">
         <v>-0.806451612903226</v>
       </c>
-      <c r="Q84" t="n">
+      <c r="R84" t="n">
         <v>-1.0</v>
       </c>
-      <c r="R84" t="n">
-        <v>3.0</v>
-      </c>
       <c r="S84" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="T84" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="U84" t="n">
         <v>1.14285714285714</v>
       </c>
-      <c r="U84" t="n">
-        <v>1.0</v>
-      </c>
       <c r="V84" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W84" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X84" t="n">
         <v>-0.125</v>
       </c>
-      <c r="X84" t="n">
+      <c r="Y84" t="n">
         <v>-0.125</v>
       </c>
     </row>
@@ -6394,33 +6649,36 @@
         <v>0.0</v>
       </c>
       <c r="O85" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P85" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q85" t="n">
         <v>-0.714285714285715</v>
       </c>
-      <c r="Q85" t="n">
+      <c r="R85" t="n">
         <v>-0.518987341772152</v>
       </c>
-      <c r="R85" t="n">
+      <c r="S85" t="n">
         <v>6.0</v>
       </c>
-      <c r="S85" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T85" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U85" t="n">
         <v>1.58333333333333</v>
       </c>
-      <c r="U85" t="n">
+      <c r="V85" t="n">
         <v>0.694776714513557</v>
       </c>
-      <c r="V85" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W85" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X85" t="n">
         <v>0.6</v>
       </c>
-      <c r="X85" t="n">
+      <c r="Y85" t="n">
         <v>1.5</v>
       </c>
     </row>
@@ -6468,33 +6726,36 @@
         <v>0.0</v>
       </c>
       <c r="O86" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P86" t="n">
         <v>0.758620689655172</v>
       </c>
-      <c r="P86" t="n">
+      <c r="Q86" t="n">
         <v>0.0991865059519849</v>
       </c>
-      <c r="Q86" t="n">
+      <c r="R86" t="n">
         <v>-0.709578188811821</v>
       </c>
-      <c r="R86" t="n">
-        <v>3.0</v>
-      </c>
       <c r="S86" t="n">
         <v>3.0</v>
       </c>
       <c r="T86" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="U86" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V86" t="n">
         <v>0.850325113483008</v>
       </c>
-      <c r="V86" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W86" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X86" t="n">
         <v>-0.461538461538462</v>
       </c>
-      <c r="X86" t="n">
+      <c r="Y86" t="n">
         <v>-1.38461538461538</v>
       </c>
     </row>
@@ -6542,26 +6803,26 @@
         <v>5.0</v>
       </c>
       <c r="O87" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P87" t="n">
         <v>0.8</v>
       </c>
-      <c r="P87" t="n">
+      <c r="Q87" t="n">
         <v>-0.597614304667197</v>
       </c>
-      <c r="Q87" t="n">
+      <c r="R87" t="n">
         <v>-0.25</v>
       </c>
-      <c r="R87" t="n">
-        <v>3.0</v>
-      </c>
       <c r="S87" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="T87" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U87" t="n">
         <v>1.8</v>
       </c>
-      <c r="U87" t="n">
-        <v>0.0</v>
-      </c>
       <c r="V87" t="n">
         <v>0.0</v>
       </c>
@@ -6569,6 +6830,9 @@
         <v>0.0</v>
       </c>
       <c r="X87" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y87" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -6616,33 +6880,36 @@
         <v>4.0</v>
       </c>
       <c r="O88" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P88" t="n">
         <v>0.714285714285714</v>
       </c>
-      <c r="P88" t="n">
+      <c r="Q88" t="n">
         <v>-0.637925343915763</v>
       </c>
-      <c r="Q88" t="n">
+      <c r="R88" t="n">
         <v>-1.0</v>
       </c>
-      <c r="R88" t="n">
+      <c r="S88" t="n">
         <v>5.0</v>
       </c>
-      <c r="S88" t="n">
-        <v>2.0</v>
-      </c>
       <c r="T88" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="U88" t="n">
         <v>1.57142857142857</v>
       </c>
-      <c r="U88" t="n">
-        <v>1.0</v>
-      </c>
       <c r="V88" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W88" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X88" t="n">
         <v>0.2</v>
       </c>
-      <c r="X88" t="n">
+      <c r="Y88" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -6690,33 +6957,36 @@
         <v>2.0</v>
       </c>
       <c r="O89" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P89" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q89" t="n">
         <v>-0.70873786407767</v>
       </c>
-      <c r="Q89" t="n">
+      <c r="R89" t="n">
         <v>-0.6</v>
       </c>
-      <c r="R89" t="n">
+      <c r="S89" t="n">
         <v>7.0</v>
       </c>
-      <c r="S89" t="n">
-        <v>3.0</v>
-      </c>
       <c r="T89" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="U89" t="n">
         <v>2.375</v>
       </c>
-      <c r="U89" t="n">
+      <c r="V89" t="n">
         <v>0.673015873015873</v>
       </c>
-      <c r="V89" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W89" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X89" t="n">
         <v>-0.285714285714286</v>
       </c>
-      <c r="X89" t="n">
+      <c r="Y89" t="n">
         <v>-0.714285714285714</v>
       </c>
     </row>
@@ -6764,33 +7034,36 @@
         <v>2.0</v>
       </c>
       <c r="O90" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P90" t="n">
         <v>0.625</v>
       </c>
-      <c r="P90" t="n">
+      <c r="Q90" t="n">
         <v>-0.0126582278481013</v>
       </c>
-      <c r="Q90" t="n">
+      <c r="R90" t="n">
         <v>-0.190300786083424</v>
       </c>
-      <c r="R90" t="n">
+      <c r="S90" t="n">
         <v>7.0</v>
       </c>
-      <c r="S90" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T90" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U90" t="n">
         <v>1.875</v>
       </c>
-      <c r="U90" t="n">
+      <c r="V90" t="n">
         <v>0.648476523476524</v>
       </c>
-      <c r="V90" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W90" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X90" t="n">
         <v>-0.333333333333333</v>
       </c>
-      <c r="X90" t="n">
+      <c r="Y90" t="n">
         <v>-1.11111111111111</v>
       </c>
     </row>
@@ -6838,33 +7111,36 @@
         <v>6.0</v>
       </c>
       <c r="O91" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P91" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="P91" t="n">
+      <c r="Q91" t="n">
         <v>-0.699999999999999</v>
       </c>
-      <c r="Q91" t="n">
+      <c r="R91" t="n">
         <v>-1.0</v>
       </c>
-      <c r="R91" t="n">
-        <v>4.0</v>
-      </c>
       <c r="S91" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="T91" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="U91" t="n">
         <v>1.22222222222222</v>
       </c>
-      <c r="U91" t="n">
-        <v>1.0</v>
-      </c>
       <c r="V91" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W91" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X91" t="n">
         <v>-0.142857142857143</v>
       </c>
-      <c r="X91" t="n">
+      <c r="Y91" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -6912,33 +7188,36 @@
         <v>6.0</v>
       </c>
       <c r="O92" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P92" t="n">
         <v>0.947368421052632</v>
       </c>
-      <c r="P92" t="n">
+      <c r="Q92" t="n">
         <v>0.344827586206897</v>
       </c>
-      <c r="Q92" t="n">
+      <c r="R92" t="n">
         <v>-0.530555555555555</v>
       </c>
-      <c r="R92" t="n">
+      <c r="S92" t="n">
         <v>6.0</v>
       </c>
-      <c r="S92" t="n">
-        <v>4.0</v>
-      </c>
       <c r="T92" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U92" t="n">
         <v>1.21052631578947</v>
       </c>
-      <c r="U92" t="n">
+      <c r="V92" t="n">
         <v>0.632031857031857</v>
       </c>
-      <c r="V92" t="n">
-        <v>0.0</v>
-      </c>
       <c r="W92" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X92" t="n">
         <v>-0.1</v>
       </c>
-      <c r="X92" t="n">
+      <c r="Y92" t="n">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add invalid dashed edges column
</commit_message>
<xml_diff>
--- a/data/study2canada_indicatorsCAMs_long.xlsx
+++ b/data/study2canada_indicatorsCAMs_long.xlsx
@@ -412,7 +412,7 @@
         <v>11.0</v>
       </c>
       <c r="O4" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="P4" t="n">
         <v>0.545454545454545</v>
@@ -566,7 +566,7 @@
         <v>8.0</v>
       </c>
       <c r="O6" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="P6" t="n">
         <v>0.5</v>
@@ -797,7 +797,7 @@
         <v>4.0</v>
       </c>
       <c r="O9" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="P9" t="n">
         <v>1.0</v>
@@ -951,7 +951,7 @@
         <v>5.0</v>
       </c>
       <c r="O11" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="P11" t="n">
         <v>0.857142857142857</v>
@@ -1336,7 +1336,7 @@
         <v>1.0</v>
       </c>
       <c r="O16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P16" t="n">
         <v>0.0</v>
@@ -1413,7 +1413,7 @@
         <v>2.0</v>
       </c>
       <c r="O17" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="P17" t="n">
         <v>0.6</v>
@@ -1490,7 +1490,7 @@
         <v>5.0</v>
       </c>
       <c r="O18" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="P18" t="n">
         <v>0.0833333333333333</v>
@@ -1567,7 +1567,7 @@
         <v>6.0</v>
       </c>
       <c r="O19" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="P19" t="n">
         <v>0.6875</v>
@@ -1644,7 +1644,7 @@
         <v>1.0</v>
       </c>
       <c r="O20" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P20" t="n">
         <v>0.307692307692308</v>
@@ -1798,7 +1798,7 @@
         <v>2.0</v>
       </c>
       <c r="O22" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="P22" t="n">
         <v>0.869565217391304</v>
@@ -1875,7 +1875,7 @@
         <v>6.0</v>
       </c>
       <c r="O23" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="P23" t="n">
         <v>1.0</v>
@@ -1952,7 +1952,7 @@
         <v>3.0</v>
       </c>
       <c r="O24" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="P24" t="n">
         <v>0.4</v>
@@ -2029,7 +2029,7 @@
         <v>2.0</v>
       </c>
       <c r="O25" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="P25" t="n">
         <v>0.428571428571429</v>
@@ -2183,7 +2183,7 @@
         <v>4.0</v>
       </c>
       <c r="O27" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P27" t="n">
         <v>0.222222222222222</v>
@@ -2337,7 +2337,7 @@
         <v>11.0</v>
       </c>
       <c r="O29" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="P29" t="n">
         <v>0.628571428571429</v>
@@ -2568,7 +2568,7 @@
         <v>14.0</v>
       </c>
       <c r="O32" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="P32" t="n">
         <v>0.904761904761905</v>
@@ -2876,7 +2876,7 @@
         <v>5.0</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P36" t="n">
         <v>0.416666666666667</v>
@@ -2953,7 +2953,7 @@
         <v>4.0</v>
       </c>
       <c r="O37" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P37" t="n">
         <v>0.545454545454545</v>
@@ -3338,7 +3338,7 @@
         <v>6.0</v>
       </c>
       <c r="O42" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="P42" t="n">
         <v>0.923076923076923</v>
@@ -3415,7 +3415,7 @@
         <v>4.0</v>
       </c>
       <c r="O43" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="P43" t="n">
         <v>0.888888888888889</v>
@@ -3492,7 +3492,7 @@
         <v>13.0</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="P44" t="n">
         <v>0.645161290322581</v>
@@ -3646,7 +3646,7 @@
         <v>12.0</v>
       </c>
       <c r="O46" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="P46" t="n">
         <v>0.588235294117647</v>
@@ -3800,7 +3800,7 @@
         <v>3.0</v>
       </c>
       <c r="O48" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="P48" t="n">
         <v>0.133333333333333</v>
@@ -3954,7 +3954,7 @@
         <v>5.0</v>
       </c>
       <c r="O50" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="P50" t="n">
         <v>0.782608695652174</v>
@@ -4031,7 +4031,7 @@
         <v>4.0</v>
       </c>
       <c r="O51" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="P51" t="n">
         <v>0.666666666666667</v>
@@ -4108,7 +4108,7 @@
         <v>20.0</v>
       </c>
       <c r="O52" t="n">
-        <v>14.0</v>
+        <v>2.0</v>
       </c>
       <c r="P52" t="n">
         <v>0.986666666666667</v>
@@ -4262,7 +4262,7 @@
         <v>2.0</v>
       </c>
       <c r="O54" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="P54" t="n">
         <v>1.0</v>
@@ -4339,7 +4339,7 @@
         <v>6.0</v>
       </c>
       <c r="O55" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="P55" t="n">
         <v>0.777777777777778</v>
@@ -4416,7 +4416,7 @@
         <v>6.0</v>
       </c>
       <c r="O56" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="P56" t="n">
         <v>0.181818181818182</v>
@@ -4570,7 +4570,7 @@
         <v>15.0</v>
       </c>
       <c r="O58" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="P58" t="n">
         <v>0.476190476190476</v>
@@ -4647,7 +4647,7 @@
         <v>1.0</v>
       </c>
       <c r="O59" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P59" t="n">
         <v>0.0</v>
@@ -4724,7 +4724,7 @@
         <v>5.0</v>
       </c>
       <c r="O60" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="P60" t="n">
         <v>0.952380952380952</v>
@@ -4801,7 +4801,7 @@
         <v>6.0</v>
       </c>
       <c r="O61" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="P61" t="n">
         <v>1.0</v>
@@ -4878,7 +4878,7 @@
         <v>18.0</v>
       </c>
       <c r="O62" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="P62" t="n">
         <v>0.72</v>
@@ -5109,7 +5109,7 @@
         <v>2.0</v>
       </c>
       <c r="O65" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="P65" t="n">
         <v>0.727272727272727</v>
@@ -5263,7 +5263,7 @@
         <v>20.0</v>
       </c>
       <c r="O67" t="n">
-        <v>6.0</v>
+        <v>12.0</v>
       </c>
       <c r="P67" t="n">
         <v>0.6875</v>
@@ -5648,7 +5648,7 @@
         <v>2.0</v>
       </c>
       <c r="O72" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="P72" t="n">
         <v>0.769230769230769</v>
@@ -5879,7 +5879,7 @@
         <v>2.0</v>
       </c>
       <c r="O75" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="P75" t="n">
         <v>0.444444444444444</v>
@@ -6033,7 +6033,7 @@
         <v>6.0</v>
       </c>
       <c r="O77" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="P77" t="n">
         <v>1.0</v>
@@ -6341,7 +6341,7 @@
         <v>7.0</v>
       </c>
       <c r="O81" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="P81" t="n">
         <v>0.893617021276596</v>
@@ -6495,7 +6495,7 @@
         <v>1.0</v>
       </c>
       <c r="O83" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P83" t="n">
         <v>0.8</v>
@@ -6803,7 +6803,7 @@
         <v>5.0</v>
       </c>
       <c r="O87" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P87" t="n">
         <v>0.8</v>
@@ -6957,7 +6957,7 @@
         <v>2.0</v>
       </c>
       <c r="O89" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="P89" t="n">
         <v>1.0</v>
@@ -7034,7 +7034,7 @@
         <v>2.0</v>
       </c>
       <c r="O90" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="P90" t="n">
         <v>0.625</v>
@@ -7188,7 +7188,7 @@
         <v>6.0</v>
       </c>
       <c r="O92" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="P92" t="n">
         <v>0.947368421052632</v>

</xml_diff>